<commit_message>
gantt-chart & powerbi file
</commit_message>
<xml_diff>
--- a/working_files_ruta/Agile_Gantt_chart.xlsx
+++ b/working_files_ruta/Agile_Gantt_chart.xlsx
@@ -3,22 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="461" documentId="8_{A84FA002-DAE3-4EA6-9FFA-1110F0DD3C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D0C5255-FCF9-4828-B8C6-E72D778BFC09}"/>
+  <xr:revisionPtr revIDLastSave="554" documentId="8_{A84FA002-DAE3-4EA6-9FFA-1110F0DD3C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85059B9D-7EB8-417A-93D6-DCC1ACF08894}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Light" sheetId="17" r:id="rId1"/>
     <sheet name="Copy for printing" sheetId="18" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Copy for printing'!$A$1:$W$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Copy for printing'!$A$1:$U$32</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Light!$A$1:$AK$33</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Copy for printing'!$6:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Copy for printing'!$7:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Light!$6:$9</definedName>
     <definedName name="Project_Start" localSheetId="1">'Copy for printing'!$D$6</definedName>
     <definedName name="Project_Start" localSheetId="0">Light!$D$6</definedName>
-    <definedName name="Scrolling_Increment" localSheetId="1">'Copy for printing'!$C$7</definedName>
+    <definedName name="Scrolling_Increment" localSheetId="1">'Copy for printing'!#REF!</definedName>
     <definedName name="Scrolling_Increment" localSheetId="0">Light!$C$7</definedName>
     <definedName name="Today" localSheetId="1">TODAY()</definedName>
     <definedName name="Today" localSheetId="0">TODAY()</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="68">
   <si>
     <t>Project Start Date:</t>
   </si>
@@ -217,6 +217,39 @@
   </si>
   <si>
     <t>avril</t>
+  </si>
+  <si>
+    <t>mai</t>
+  </si>
+  <si>
+    <t>np, plt, px</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Flask, joblib</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
   </si>
 </sst>
 </file>
@@ -652,7 +685,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -872,6 +905,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -938,7 +989,7 @@
     <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1083,6 +1134,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1098,11 +1158,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1157,7 +1217,123 @@
     <cellStyle name="Warning Text" xfId="23" builtinId="11" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="54">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1215,16 +1391,41 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
       <border>
         <left/>
         <right/>
         <top/>
-        <bottom/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1277,61 +1478,6 @@
         <bottom style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1401,41 +1547,6 @@
         <right/>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1599,27 +1710,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.249977111117893"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1920,21 +2010,21 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gantt Table Style" pivot="0" count="4" xr9:uid="{4904D139-63E4-4221-B7C9-C6C5B7A50FAF}">
-      <tableStyleElement type="wholeTable" dxfId="51"/>
-      <tableStyleElement type="headerRow" dxfId="50"/>
-      <tableStyleElement type="firstRowStripe" dxfId="49"/>
-      <tableStyleElement type="secondRowStripe" dxfId="48"/>
+      <tableStyleElement type="wholeTable" dxfId="53"/>
+      <tableStyleElement type="headerRow" dxfId="52"/>
+      <tableStyleElement type="firstRowStripe" dxfId="51"/>
+      <tableStyleElement type="secondRowStripe" dxfId="50"/>
     </tableStyle>
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="47"/>
-      <tableStyleElement type="headerRow" dxfId="46"/>
-      <tableStyleElement type="totalRow" dxfId="45"/>
-      <tableStyleElement type="firstColumn" dxfId="44"/>
-      <tableStyleElement type="lastColumn" dxfId="43"/>
-      <tableStyleElement type="firstRowStripe" dxfId="42"/>
-      <tableStyleElement type="secondRowStripe" dxfId="41"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="40"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="39"/>
+      <tableStyleElement type="wholeTable" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="48"/>
+      <tableStyleElement type="totalRow" dxfId="47"/>
+      <tableStyleElement type="firstColumn" dxfId="46"/>
+      <tableStyleElement type="lastColumn" dxfId="45"/>
+      <tableStyleElement type="firstRowStripe" dxfId="44"/>
+      <tableStyleElement type="secondRowStripe" dxfId="43"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="42"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="41"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2031,10 +2121,6 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$C$7" horiz="1" max="365" page="2" val="0"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$C$7" horiz="1" max="365" page="2" val="0"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2090,67 +2176,12 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>31750</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>31750</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>21</xdr:col>
-          <xdr:colOff>232535</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>223592</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="17409" name="Scroll Bar 1" descr="Scroll bar to scroll through the Ghantt project timeline." hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s17409"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB6CFAEE-B78C-40F9-8B55-E8513F3C5F35}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:H32" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:H32" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="B9:H32" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2161,13 +2192,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Milestone description" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Category" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progress" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="32" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Days" dataDxfId="31" dataCellStyle="Comma [0]"/>
-    <tableColumn id="7" xr3:uid="{0B6C7F6D-8017-428A-BD17-95356BBCA3D9}" name="Material" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Milestone description" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Category" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progress" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="34" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Days" dataDxfId="33" dataCellStyle="Comma [0]"/>
+    <tableColumn id="7" xr3:uid="{0B6C7F6D-8017-428A-BD17-95356BBCA3D9}" name="Material" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2179,8 +2210,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D50C9E70-4622-4A16-8F00-8E8097379F07}" name="Milestones43523" displayName="Milestones43523" ref="B9:H32" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="B9:H32" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D50C9E70-4622-4A16-8F00-8E8097379F07}" name="Milestones43523" displayName="Milestones43523" ref="B9:H31" totalsRowShown="0" dataDxfId="31">
+  <autoFilter ref="B9:H31" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2190,13 +2221,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{427ADF16-1558-4375-8C9D-B35F514B3ECD}" name="Milestone description" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{AC340651-0C21-4DCB-98AC-A9291BEBAE19}" name="Category" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{10ECADC7-FFBD-4A4E-82DB-5CE85C9C1BE4}" name="Assigned to" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{794F5674-263F-4743-89AB-037129632D9E}" name="Progress" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{F44290BF-64E1-421A-8643-611AEFE274FD}" name="Start" dataDxfId="23" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{5647E7EC-06CB-4110-AB00-69380C3630AA}" name="Days" dataDxfId="22" dataCellStyle="Comma [0]"/>
-    <tableColumn id="7" xr3:uid="{2CD06E7C-D667-4B56-B25E-34B149C3F376}" name="Material" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{427ADF16-1558-4375-8C9D-B35F514B3ECD}" name="Column1" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{AC340651-0C21-4DCB-98AC-A9291BEBAE19}" name="Column2" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{10ECADC7-FFBD-4A4E-82DB-5CE85C9C1BE4}" name="Column3" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{794F5674-263F-4743-89AB-037129632D9E}" name="Column4" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{F44290BF-64E1-421A-8643-611AEFE274FD}" name="Column5" dataDxfId="26" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{5647E7EC-06CB-4110-AB00-69380C3630AA}" name="Column6" dataDxfId="25" dataCellStyle="Comma [0]"/>
+    <tableColumn id="7" xr3:uid="{2CD06E7C-D667-4B56-B25E-34B149C3F376}" name="Column7" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2475,7 +2506,7 @@
   </sheetPr>
   <dimension ref="A1:AJ36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="71" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" showRuler="0" zoomScale="71" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -2497,28 +2528,28 @@
     <row r="1" spans="1:36" ht="25.15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:36" s="51" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="49"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
       <c r="V2" s="50"/>
       <c r="W2" s="50"/>
       <c r="X2" s="50"/>
@@ -5345,16 +5376,16 @@
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="58" t="s">
         <v>54</v>
       </c>
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="55"/>
+      <c r="B35" s="58"/>
     </row>
     <row r="36" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="55"/>
+      <c r="B36" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5378,43 +5409,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:AI32">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>AND(TODAY()&gt;=J$7,TODAY()&lt;K$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:AJ6">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>AND(J$7&lt;=EOMONTH($J$7,1),J$7&gt;EOMONTH($J$7,0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>J$7&lt;=EOMONTH($J$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J10:AJ32">
+    <cfRule type="expression" dxfId="20" priority="157" stopIfTrue="1">
+      <formula>AND($C10="Low Risk",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="158" stopIfTrue="1">
+      <formula>AND($C10="High Risk",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="159" stopIfTrue="1">
+      <formula>AND($C10="On Track",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="160" stopIfTrue="1">
+      <formula>AND($C10="Med Risk",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="161" stopIfTrue="1">
+      <formula>AND(LEN($C10)=0,J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K6:AJ6">
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>AND(K$7&lt;=EOMONTH($J$7,2),K$7&gt;EOMONTH($J$7,0),K$7&gt;EOMONTH($J$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ7:AJ32">
-    <cfRule type="expression" dxfId="16" priority="91">
+    <cfRule type="expression" dxfId="14" priority="91">
       <formula>AND(TODAY()&gt;=AJ$7,TODAY()&lt;#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:AJ32">
-    <cfRule type="expression" dxfId="15" priority="157" stopIfTrue="1">
-      <formula>AND($C10="Low Risk",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="158" stopIfTrue="1">
-      <formula>AND($C10="High Risk",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="159" stopIfTrue="1">
-      <formula>AND($C10="On Track",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="160" stopIfTrue="1">
-      <formula>AND($C10="Med Risk",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="161" stopIfTrue="1">
-      <formula>AND(LEN($C10)=0,J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="12">
@@ -5520,10 +5551,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScale="71" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A21" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="U35" sqref="B2:U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5537,38 +5568,36 @@
     <col min="7" max="7" width="8.7265625" customWidth="1"/>
     <col min="8" max="8" width="17.90625" customWidth="1"/>
     <col min="9" max="9" width="2.7265625" customWidth="1"/>
-    <col min="10" max="22" width="3.54296875" customWidth="1"/>
-    <col min="24" max="24" width="8.81640625" customWidth="1"/>
+    <col min="10" max="21" width="3.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="25.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:23" s="51" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="25.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:21" s="51" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="49"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="50"/>
       <c r="P2" s="50"/>
       <c r="Q2" s="50"/>
       <c r="R2" s="50"/>
       <c r="S2" s="50"/>
       <c r="T2" s="50"/>
       <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
     </row>
-    <row r="3" spans="1:23" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="21"/>
       <c r="C3" s="22"/>
@@ -5576,7 +5605,7 @@
       <c r="E3" s="23"/>
       <c r="F3" s="24"/>
     </row>
-    <row r="4" spans="1:23" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
       <c r="B4" s="25" t="s">
         <v>10</v>
@@ -5586,7 +5615,7 @@
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
     </row>
-    <row r="5" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="45" t="s">
         <v>11</v>
@@ -5599,7 +5628,7 @@
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
     </row>
-    <row r="6" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="30" t="s">
         <v>0</v>
@@ -5612,167 +5641,120 @@
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
-      <c r="J6" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
     </row>
-    <row r="7" spans="1:23" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
-      <c r="B7" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="47">
-        <v>0</v>
-      </c>
-      <c r="D7" s="27"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="38">
+      <c r="I7" s="28"/>
+      <c r="J7" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="U7" s="34"/>
+    </row>
+    <row r="8" spans="1:21" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="32"/>
+      <c r="J8" s="38">
         <v>45376</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K8" s="39">
         <v>45377</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L8" s="39">
         <v>45378</v>
       </c>
-      <c r="M7" s="39">
+      <c r="M8" s="39">
         <v>45379</v>
       </c>
-      <c r="N7" s="39">
+      <c r="N8" s="39">
         <v>45380</v>
       </c>
-      <c r="O7" s="39">
-        <v>45381</v>
-      </c>
-      <c r="P7" s="40">
-        <v>45382</v>
-      </c>
-      <c r="Q7" s="39">
+      <c r="O8" s="39">
         <v>45397</v>
       </c>
-      <c r="R7" s="39">
+      <c r="P8" s="39">
         <v>45398</v>
       </c>
-      <c r="S7" s="39">
+      <c r="Q8" s="39">
         <v>45399</v>
       </c>
-      <c r="T7" s="39">
+      <c r="R8" s="39">
         <v>45400</v>
       </c>
-      <c r="U7" s="39">
+      <c r="S8" s="39">
         <v>45401</v>
       </c>
-      <c r="V7" s="39">
-        <v>45402</v>
+      <c r="T8" s="39">
+        <v>45418</v>
+      </c>
+      <c r="U8" s="39">
+        <v>45419</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
+    <row r="9" spans="1:21" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="53"/>
     </row>
-    <row r="9" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="33"/>
-      <c r="J9" s="38">
-        <v>45376</v>
-      </c>
-      <c r="K9" s="39">
-        <v>45377</v>
-      </c>
-      <c r="L9" s="39">
-        <v>45378</v>
-      </c>
-      <c r="M9" s="39">
-        <v>45379</v>
-      </c>
-      <c r="N9" s="39">
-        <v>45380</v>
-      </c>
-      <c r="O9" s="39">
-        <v>45381</v>
-      </c>
-      <c r="P9" s="40">
-        <v>45382</v>
-      </c>
-      <c r="Q9" s="39">
-        <v>45397</v>
-      </c>
-      <c r="R9" s="39">
-        <v>45398</v>
-      </c>
-      <c r="S9" s="39">
-        <v>45399</v>
-      </c>
-      <c r="T9" s="39">
-        <v>45400</v>
-      </c>
-      <c r="U9" s="39">
-        <v>45401</v>
-      </c>
-      <c r="V9" s="39">
-        <v>45402</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
       <c r="C10" s="10"/>
       <c r="D10" s="9"/>
@@ -5792,9 +5774,8 @@
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
     </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="37" t="s">
         <v>13</v>
@@ -5805,25 +5786,25 @@
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="56"/>
-      <c r="T11" s="56"/>
-      <c r="U11" s="56"/>
-      <c r="V11" s="56"/>
-      <c r="W11" s="58"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="61"/>
+      <c r="S11" s="61"/>
+      <c r="T11" s="61"/>
+      <c r="U11" s="54" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="20" t="s">
         <v>29</v>
@@ -5859,9 +5840,8 @@
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
     </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="20" t="s">
         <v>26</v>
@@ -5921,11 +5901,8 @@
       <c r="U13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="V13" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="20" t="s">
         <v>28</v>
@@ -5961,9 +5938,8 @@
       <c r="S14" s="14"/>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="20" t="s">
         <v>27</v>
@@ -5999,9 +5975,8 @@
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
       <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
     </row>
-    <row r="16" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="20" t="s">
         <v>34</v>
@@ -6037,9 +6012,8 @@
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
       <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
     </row>
-    <row r="17" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="37" t="s">
         <v>12</v>
@@ -6050,25 +6024,25 @@
       <c r="F17" s="18"/>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="56"/>
-      <c r="T17" s="56"/>
-      <c r="U17" s="56"/>
-      <c r="V17" s="56"/>
-      <c r="W17" s="58"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="59"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="52" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="20" t="s">
         <v>18</v>
@@ -6128,11 +6102,8 @@
       <c r="U18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="V18" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="19" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="20" t="s">
         <v>47</v>
@@ -6192,11 +6163,8 @@
       <c r="U19" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="V19" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="20" t="s">
         <v>19</v>
@@ -6211,13 +6179,13 @@
         <v>1</v>
       </c>
       <c r="F20" s="18">
-        <v>45381</v>
+        <v>45397</v>
       </c>
       <c r="G20" s="19">
         <v>1</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="14" t="s">
@@ -6256,11 +6224,8 @@
       <c r="U20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="V20" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="21" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="20" t="s">
         <v>20</v>
@@ -6278,7 +6243,7 @@
         <v>45397</v>
       </c>
       <c r="G21" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21" s="19" t="s">
         <v>39</v>
@@ -6320,11 +6285,8 @@
       <c r="U21" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="V21" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="22" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="37" t="s">
         <v>14</v>
@@ -6335,25 +6297,25 @@
       <c r="F22" s="18"/>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="56"/>
-      <c r="S22" s="56"/>
-      <c r="T22" s="56"/>
-      <c r="U22" s="56"/>
-      <c r="V22" s="56"/>
-      <c r="W22" s="58"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="59"/>
+      <c r="T22" s="59"/>
+      <c r="U22" s="52" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="20" t="s">
         <v>36</v>
@@ -6371,10 +6333,10 @@
         <v>45397</v>
       </c>
       <c r="G23" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="I23" s="16"/>
       <c r="J23" s="14"/>
@@ -6389,9 +6351,8 @@
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
       <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
     </row>
-    <row r="24" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="20" t="s">
         <v>48</v>
@@ -6400,16 +6361,18 @@
         <v>4</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="18">
-        <v>45397</v>
+        <v>45398</v>
       </c>
       <c r="G24" s="19">
         <v>3</v>
       </c>
-      <c r="H24" s="19"/>
+      <c r="H24" s="19" t="s">
+        <v>53</v>
+      </c>
       <c r="I24" s="16"/>
       <c r="J24" s="14" t="s">
         <v>42</v>
@@ -6447,11 +6410,8 @@
       <c r="U24" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="V24" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="25" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="20" t="s">
         <v>43</v>
@@ -6460,14 +6420,14 @@
         <v>4</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="18">
         <v>45399</v>
       </c>
       <c r="G25" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>53</v>
@@ -6509,119 +6469,115 @@
       <c r="U25" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="V25" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="26" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
-      <c r="B26" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="B26" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="18">
-        <v>45399</v>
-      </c>
-      <c r="G26" s="19">
-        <v>1</v>
-      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19"/>
       <c r="H26" s="19"/>
       <c r="I26" s="16"/>
-      <c r="J26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="M26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="N26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="O26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="P26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="R26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="S26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="T26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="U26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="V26" s="14" t="s">
+      <c r="J26" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="52" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
-      <c r="B27" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="B27" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="K27" s="56"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-      <c r="O27" s="56"/>
-      <c r="P27" s="56"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="56"/>
-      <c r="S27" s="56"/>
-      <c r="T27" s="56"/>
-      <c r="U27" s="56"/>
-      <c r="V27" s="56"/>
-      <c r="W27" s="58"/>
+      <c r="F27" s="18">
+        <v>45400</v>
+      </c>
+      <c r="G27" s="19">
+        <v>2</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="16"/>
+      <c r="J27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="N27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="O27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="P27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="R27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="S27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="T27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="U27" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="28" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="18">
-        <v>45400</v>
+        <v>45418</v>
       </c>
       <c r="G28" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I28" s="16"/>
       <c r="J28" s="14" t="s">
@@ -6660,105 +6616,99 @@
       <c r="U28" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="V28" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="29" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
-      <c r="B29" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="16" t="s">
+      <c r="B29" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="K29" s="59"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="59"/>
+      <c r="R29" s="59"/>
+      <c r="S29" s="59"/>
+      <c r="T29" s="60"/>
+      <c r="U29" s="52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="6"/>
+      <c r="B30" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18">
-        <v>45400</v>
-      </c>
-      <c r="G29" s="19">
-        <v>2</v>
-      </c>
-      <c r="H29" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="16"/>
-      <c r="J29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="M29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="N29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="O29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="P29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="R29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="S29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="T29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="U29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="V29" s="14" t="s">
+      <c r="D30" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18">
+        <v>45418</v>
+      </c>
+      <c r="G30" s="19">
+        <v>1</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="16"/>
+      <c r="J30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="N30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="O30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="P30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="R30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="S30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="T30" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="U30" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
-      <c r="B30" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="K30" s="56"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="56"/>
-      <c r="S30" s="56"/>
-      <c r="T30" s="56"/>
-      <c r="U30" s="56"/>
-      <c r="V30" s="56"/>
-      <c r="W30" s="58"/>
-    </row>
-    <row r="31" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>4</v>
@@ -6768,13 +6718,13 @@
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="18">
-        <v>45401</v>
+        <v>45418</v>
       </c>
       <c r="G31" s="19">
         <v>1</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I31" s="16"/>
       <c r="J31" s="14" t="s">
@@ -6813,103 +6763,38 @@
       <c r="U31" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="V31" s="14" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="32" spans="1:23" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6"/>
-      <c r="B32" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="18">
-        <v>45401</v>
-      </c>
-      <c r="G32" s="19">
-        <v>1</v>
-      </c>
-      <c r="H32" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="I32" s="16"/>
-      <c r="J32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="M32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="N32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="O32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="P32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="R32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="S32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="T32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="U32" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="V32" s="14" t="s">
-        <v>42</v>
-      </c>
+    <row r="32" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D32" s="4"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D33" s="4"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="3"/>
+    <row r="33" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="5"/>
+    <row r="34" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="58"/>
     </row>
-    <row r="35" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="55"/>
-    </row>
-    <row r="36" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="55"/>
+    <row r="35" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="J30:V30"/>
-    <mergeCell ref="J27:V27"/>
-    <mergeCell ref="J22:V22"/>
-    <mergeCell ref="J17:V17"/>
-    <mergeCell ref="J11:V11"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="J29:T29"/>
+    <mergeCell ref="J26:T26"/>
+    <mergeCell ref="J22:T22"/>
+    <mergeCell ref="J17:T17"/>
+    <mergeCell ref="J11:T11"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E32">
-    <cfRule type="dataBar" priority="5">
+  <conditionalFormatting sqref="E10:E31 E8">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6922,105 +6807,89 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:O10 Q7:U10 Q31:U32 J31:O32 J30 Q28:U29 J28:O29 J27 Q23:U26 J23:O26 J22 Q18:U21 J18:O21 J17 Q12:U16 J12:O16 J11">
-    <cfRule type="expression" dxfId="10" priority="1">
-      <formula>AND(TODAY()&gt;=J$7,TODAY()&lt;K$7)</formula>
+  <conditionalFormatting sqref="J8:M8 O8:S8 J10:M10 O10:S10 J11 J12:M16 O12:S16 J17 J18:M21 O18:S21 J22 J23:M25 O23:S25 J26 J27:M28 O27:S28 J29 J30:M31">
+    <cfRule type="expression" dxfId="13" priority="12">
+      <formula>AND(TODAY()&gt;=J$8,TODAY()&lt;K$8)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6:V6">
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>AND(J$7&lt;=EOMONTH($J$7,1),J$7&gt;EOMONTH($J$7,0))</formula>
+  <conditionalFormatting sqref="J7:U7">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>AND(J$8&lt;=EOMONTH($J$8,1),J$8&gt;EOMONTH($J$8,0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
-      <formula>J$7&lt;=EOMONTH($J$7,0)</formula>
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>J$8&lt;=EOMONTH($J$8,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:V6">
-    <cfRule type="expression" dxfId="7" priority="3">
-      <formula>AND(K$7&lt;=EOMONTH($J$7,2),K$7&gt;EOMONTH($J$7,0),K$7&gt;EOMONTH($J$7,1))</formula>
+  <conditionalFormatting sqref="J10:U10 J11 J12:U16 J17 J18:U21 J22 J23:U25 J26 J27:U28 J29 J30:U31">
+    <cfRule type="expression" dxfId="10" priority="184" stopIfTrue="1">
+      <formula>AND($C10="High Risk",J$8&gt;=$F10,J$8&lt;=$F10+$G10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="185" stopIfTrue="1">
+      <formula>AND($C10="On Track",J$8&gt;=$F10,J$8&lt;=$F10+$G10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="186" stopIfTrue="1">
+      <formula>AND($C10="Med Risk",J$8&gt;=$F10,J$8&lt;=$F10+$G10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="187" stopIfTrue="1">
+      <formula>AND(LEN($C10)=0,J$8&gt;=$F10,J$8&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V7:V10 V31:V32 V28:V29 V23:V26 V18:V21 V12:V16">
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>AND(TODAY()&gt;=V$7,TODAY()&lt;#REF!)</formula>
+  <conditionalFormatting sqref="J10:U10 J12:U16 J18:U21 J23:U25 J27:U28 J30:U31 J11 J17 J22 J26 J29">
+    <cfRule type="expression" dxfId="6" priority="183" stopIfTrue="1">
+      <formula>AND($C10="Low Risk",J$8&gt;=$F10,J$8&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P7:P10 P31:P32 P28:P29 P23:P26 P18:P21 P12:P16">
-    <cfRule type="expression" dxfId="5" priority="164">
-      <formula>AND(TODAY()&gt;=P$7,TODAY()&lt;#REF!)</formula>
+  <conditionalFormatting sqref="K7:U7">
+    <cfRule type="expression" dxfId="5" priority="14">
+      <formula>AND(K$8&lt;=EOMONTH($J$8,2),K$8&gt;EOMONTH($J$8,0),K$8&gt;EOMONTH($J$8,1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10:V10 J31:V32 J30 J28:V29 J27 J23:V26 J22 J18:V21 J17 J12:V16 J11">
-    <cfRule type="expression" dxfId="4" priority="172" stopIfTrue="1">
-      <formula>AND($C10="Low Risk",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="173" stopIfTrue="1">
-      <formula>AND($C10="High Risk",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="174" stopIfTrue="1">
-      <formula>AND($C10="On Track",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="175" stopIfTrue="1">
-      <formula>AND($C10="Med Risk",J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="176" stopIfTrue="1">
-      <formula>AND(LEN($C10)=0,J$7&gt;=$F10,J$7&lt;=$F10+$G10-1)</formula>
+  <conditionalFormatting sqref="N10 N12:N16 N18:N21 N23:N25 N27:N28 N30:N31 N8">
+    <cfRule type="expression" dxfId="4" priority="189">
+      <formula>AND(TODAY()&gt;=N$8,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="12">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an empty row" sqref="A30:A32" xr:uid="{6E9F00C6-B6CF-4C5A-A47C-42682873110D}"/>
+  <conditionalFormatting sqref="O30:U31">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>AND(TODAY()&gt;=O$8,TODAY()&lt;P$8)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T8 T10 T12:T16 T18:T21 T23:T25 T27:T28 T30:T31">
+    <cfRule type="expression" dxfId="2" priority="17">
+      <formula>AND(TODAY()&gt;=T$8,TODAY()&lt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U8">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>AND(TODAY()&gt;=U$8,TODAY()&lt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U10 U12:U16 U18:U21 U23:U25 U27:U28 U30:U31">
+    <cfRule type="expression" dxfId="0" priority="7">
+      <formula>AND(TODAY()&gt;=U$8,TODAY()&lt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="10">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an empty row" sqref="A29:A31" xr:uid="{6E9F00C6-B6CF-4C5A-A47C-42682873110D}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Project information starting in cell B11 through cell G11. _x000a_Enter Milestone Description, select a Category, assign someone to the task, and enter the progress, start date, and number of days for the task to start charting._x000a_" sqref="A11:A13" xr:uid="{FE460384-EF1B-4803-865C-8AAE3F6677D6}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row contains headers for the project schedule.  B9 through G9 contains schedule information.  Cells I9 through BL9 contain the first letter of each day of the week for the date above that heading._x000a_All project timeline charting is auto generated." sqref="A9" xr:uid="{EB1C0D8C-A17F-4097-B096-1A2AD39E01D1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A scrollbar is in cells I8 through BL8. _x000a_To jump forward or backward in the timeline, enter a value of 0 or higher in cell C7._x000a_A value of 0 takes you to the beginning of the chart." sqref="A8" xr:uid="{F423CD7C-88D0-467A-891D-2AC7737543D6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cells I9 through BL9 contain the day number of the month for the Month represented in the cell block above each date cell and are auto calculated._x000a_Do not modify these cells._x000a_" sqref="A7" xr:uid="{61A769FD-4552-4EE3-905C-AD81C124902E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A Scrolling Increment is in cell C7. _x000a_Months for the dates in row 7 are displayed starting in cells I6 through cell BL6._x000a_Do not modify these cells. They are auto updated based on the project start date in cell F6." sqref="A6" xr:uid="{27EE7944-5244-4CE0-A0AF-9FC393A71355}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the Project Lead in cell B5. Enter the Project Start date in cell C6 or allow the sample formula to find the smallest date value from the Gantt Data table.  _x000a_Project Start Date: label is in cell B6." sqref="A5" xr:uid="{CA1A85C2-2FD9-4B4E-992A-F07CE7CA06DC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cells I9 through BL9 contain the day number of the month for the Month represented in the cell block above each date cell and are auto calculated._x000a_Do not modify these cells._x000a_" sqref="A8" xr:uid="{61A769FD-4552-4EE3-905C-AD81C124902E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A Scrolling Increment is in cell C7. _x000a_Months for the dates in row 7 are displayed starting in cells I6 through cell BL6._x000a_Do not modify these cells. They are auto updated based on the project start date in cell F6." sqref="A7" xr:uid="{27EE7944-5244-4CE0-A0AF-9FC393A71355}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the Project Lead in cell B5. Enter the Project Start date in cell C6 or allow the sample formula to find the smallest date value from the Gantt Data table.  _x000a_Project Start Date: label is in cell B6." sqref="A5:A6" xr:uid="{CA1A85C2-2FD9-4B4E-992A-F07CE7CA06DC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Company Name in cell B4._x000a_A legend is in cells I4 through AC4.  The Legend label is in cell G4." sqref="A4" xr:uid="{352FAFCD-980C-4834-A152-428896470A52}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Create a Gantt Chart " prompt="Enter title of this project in cell B2. _x000a_Information about how to use this worksheet, including instructions for screen readers and the author of this workbook is in the About worksheet._x000a_Continue navigating down column A to hear further instructions." sqref="A2" xr:uid="{AF767375-D22E-4E29-9478-D466E1470F1C}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{65BE37CA-DB95-4DD3-A8AD-7916CFE4B468}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C32" xr:uid="{3312EE19-F5FC-4DD1-9E6E-89CB99E389B6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C31" xr:uid="{3312EE19-F5FC-4DD1-9E6E-89CB99E389B6}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="C7" xr:uid="{6F3CE484-327E-425E-82D3-1BC9E7938EA0}">
-      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="17409" r:id="rId4" name="Scroll Bar 1">
-              <controlPr defaultSize="0" autoPict="0" altText="Scroll bar to scroll through the Ghantt project timeline.">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>9</xdr:col>
-                    <xdr:colOff>31750</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>31750</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>21</xdr:col>
-                    <xdr:colOff>234950</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>222250</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -7038,10 +6907,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E32</xm:sqref>
+          <xm:sqref>E10:E31 E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="171" id="{83A918FB-495E-4E7B-964C-D6CF6C973E0A}">
+          <x14:cfRule type="iconSet" priority="297" id="{83A918FB-495E-4E7B-964C-D6CF6C973E0A}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7057,7 +6926,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>J10:V10 J31:V32 J30 J28:V29 J27 J23:V26 J22 J18:V21 J17 J12:V16 J11</xm:sqref>
+          <xm:sqref>J29 J26 J22 J17 J11 J10:U10 J27:U28 J23:U25 J18:U21 J12:U16 J30:U31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7075,25 +6944,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7369,6 +7219,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
   <ds:schemaRefs>
@@ -7378,18 +7247,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7408,4 +7265,16 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>